<commit_message>
Forsøger med industry elc restrictions
</commit_message>
<xml_diff>
--- a/TIMES-DE/SuppXLS/Scen_TRA_MIDROAD_Maxshare_Constraint.xlsx
+++ b/TIMES-DE/SuppXLS/Scen_TRA_MIDROAD_Maxshare_Constraint.xlsx
@@ -565,7 +565,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -576,7 +576,7 @@
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H9:H32"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1490,7 +1490,7 @@
         <v>38</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="N30" s="8"/>
       <c r="P30" s="7"/>
@@ -1552,7 +1552,7 @@
         <v>38</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="N32" s="8"/>
       <c r="P32" s="7"/>

</xml_diff>